<commit_message>
Revert "Merge branch 'master' of https://github.com/Hutchins-Center/Fiscal-Impact-Measure"
This reverts commit 7a61c755f0516e56c217e8fb3802a0e78f8db91a, reversing
changes made to c49a37bceb835cb150904ce5cd80d4ee5fefa1fa.
</commit_message>
<xml_diff>
--- a/data/add-ons/fim_no_addons.xlsx
+++ b/data/add-ons/fim_no_addons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scampbell\Documents\GitHub\Fiscal-Impact-Measure\data\add-ons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1210258A-DBB3-4FC2-A1DA-DF853BDBA812}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63234F9-02F6-4662-A512-8C19445B89CD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>date</t>
   </si>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I47"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection sqref="A1:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,7 +494,7 @@
         <v>156.16</v>
       </c>
       <c r="C2">
-        <v>736.59999999999991</v>
+        <v>440</v>
       </c>
       <c r="D2">
         <v>1779.8</v>
@@ -506,13 +506,13 @@
         <v>1336.74</v>
       </c>
       <c r="G2">
-        <v>3694.6000000000008</v>
+        <v>1828.5000000000009</v>
       </c>
       <c r="H2">
         <v>1085.9000000000001</v>
       </c>
       <c r="I2">
-        <v>321.35000000000002</v>
+        <v>884.2600000000001</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -523,7 +523,7 @@
         <v>197.62799999999999</v>
       </c>
       <c r="C3">
-        <v>582.79999999999995</v>
+        <v>363.8</v>
       </c>
       <c r="D3">
         <v>1871.3</v>
@@ -535,13 +535,13 @@
         <v>1328.7719999999999</v>
       </c>
       <c r="G3">
-        <v>2433.1999999999998</v>
+        <v>1861.4</v>
       </c>
       <c r="H3">
         <v>1212.9000000000001</v>
       </c>
       <c r="I3">
-        <v>291.39999999999998</v>
+        <v>242.12799999999999</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -552,7 +552,7 @@
         <v>170.20699999999999</v>
       </c>
       <c r="C4">
-        <v>341</v>
+        <v>243.1</v>
       </c>
       <c r="D4">
         <v>1907.1</v>
@@ -564,13 +564,13 @@
         <v>1372.7929999999999</v>
       </c>
       <c r="G4">
-        <v>1959.6999999999989</v>
+        <v>1756.1999999999989</v>
       </c>
       <c r="H4">
         <v>609.79999999999995</v>
       </c>
       <c r="I4">
-        <v>284.15100000000001</v>
+        <v>225.90700000000001</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -581,7 +581,7 @@
         <v>164.13699999999989</v>
       </c>
       <c r="C5">
-        <v>287.69999999999987</v>
+        <v>216.8</v>
       </c>
       <c r="D5">
         <v>1958.3</v>
@@ -593,13 +593,13 @@
         <v>1403.2629999999999</v>
       </c>
       <c r="G5">
-        <v>4215.9000000000005</v>
+        <v>1808.7</v>
       </c>
       <c r="H5">
         <v>402.3</v>
       </c>
       <c r="I5">
-        <v>357.63880399999999</v>
+        <v>260.73700000000002</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -610,7 +610,7 @@
         <v>168.2833827902208</v>
       </c>
       <c r="C6">
-        <v>249.4722454529217</v>
+        <v>201.69787045292151</v>
       </c>
       <c r="D6">
         <v>1978.3751090344099</v>
@@ -619,13 +619,13 @@
         <v>96.883099094316492</v>
       </c>
       <c r="F6">
-        <v>1561.0795271182501</v>
+        <v>1394.63952711825</v>
       </c>
       <c r="G6">
-        <v>3373.426597104331</v>
+        <v>1629.356357104331</v>
       </c>
       <c r="H6">
-        <v>567.87138158623384</v>
+        <v>404.18538158623392</v>
       </c>
       <c r="I6">
         <v>232.07518871317359</v>
@@ -639,7 +639,7 @@
         <v>172.42976558044171</v>
       </c>
       <c r="C7">
-        <v>238.93299559334321</v>
+        <v>188.86729215584299</v>
       </c>
       <c r="D7">
         <v>2007.0179878174349</v>
@@ -648,13 +648,13 @@
         <v>98.285770837814454</v>
       </c>
       <c r="F7">
-        <v>1552.4560542365</v>
+        <v>1386.0160542364999</v>
       </c>
       <c r="G7">
-        <v>2112.8103287165659</v>
+        <v>1501.6652887165669</v>
       </c>
       <c r="H7">
-        <v>569.80008156777501</v>
+        <v>406.11408156777497</v>
       </c>
       <c r="I7">
         <v>215.720203842161</v>
@@ -668,7 +668,7 @@
         <v>173.0148583315212</v>
       </c>
       <c r="C8">
-        <v>241.82759010290039</v>
+        <v>193.24899108297839</v>
       </c>
       <c r="D8">
         <v>2033.6981662082569</v>
@@ -677,13 +677,13 @@
         <v>99.592327089502035</v>
       </c>
       <c r="F8">
-        <v>1499.467429866125</v>
+        <v>1416.247429866125</v>
       </c>
       <c r="G8">
-        <v>1607.2419452477011</v>
+        <v>1514.272945247701</v>
       </c>
       <c r="H8">
-        <v>489.92497438316559</v>
+        <v>408.08197438316557</v>
       </c>
       <c r="I8">
         <v>220.89139620745101</v>
@@ -697,7 +697,7 @@
         <v>173.59995108260071</v>
       </c>
       <c r="C9">
-        <v>245.1419882747505</v>
+        <v>199.97623704208269</v>
       </c>
       <c r="D9">
         <v>2058.944408239478</v>
@@ -706,13 +706,13 @@
         <v>100.82866197730991</v>
       </c>
       <c r="F9">
-        <v>1506.8658054957491</v>
+        <v>1446.4788054957489</v>
       </c>
       <c r="G9">
-        <v>1668.6360242949511</v>
+        <v>1515.6150242949509</v>
       </c>
       <c r="H9">
-        <v>520.32055778657434</v>
+        <v>410.07255778657441</v>
       </c>
       <c r="I9">
         <v>226.76914626180869</v>
@@ -726,7 +726,7 @@
         <v>174.1850438336802</v>
       </c>
       <c r="C10">
-        <v>248.49241388178211</v>
+        <v>205.88603266163159</v>
       </c>
       <c r="D10">
         <v>2079.7902580671739</v>
@@ -735,13 +735,13 @@
         <v>101.8495050547117</v>
       </c>
       <c r="F10">
-        <v>1537.0971811253739</v>
+        <v>1476.710181125374</v>
       </c>
       <c r="G10">
-        <v>1662.947416318757</v>
+        <v>1509.926416318757</v>
       </c>
       <c r="H10">
-        <v>522.2987645056096</v>
+        <v>412.05076450560961</v>
       </c>
       <c r="I10">
         <v>232.32795235033251</v>
@@ -755,7 +755,7 @@
         <v>174.77013658475971</v>
       </c>
       <c r="C11">
-        <v>249.5444242270961</v>
+        <v>212.3326953411578</v>
       </c>
       <c r="D11">
         <v>2102.1686273791929</v>
@@ -764,13 +764,13 @@
         <v>102.94539721476001</v>
       </c>
       <c r="F11">
-        <v>1567.3285567549981</v>
+        <v>1506.9415567549979</v>
       </c>
       <c r="G11">
-        <v>1646.738834055632</v>
+        <v>1493.7178340556329</v>
       </c>
       <c r="H11">
-        <v>524.24602951371094</v>
+        <v>413.998029513711</v>
       </c>
       <c r="I11">
         <v>237.9298898973548</v>
@@ -784,7 +784,7 @@
         <v>172.87701948733081</v>
       </c>
       <c r="C12">
-        <v>259.81500173946711</v>
+        <v>229.53998058883141</v>
       </c>
       <c r="D12">
         <v>2124.2512473170441</v>
@@ -793,13 +793,13 @@
         <v>104.0268062185081</v>
       </c>
       <c r="F12">
-        <v>1580.1471557667951</v>
+        <v>1519.7601557667949</v>
       </c>
       <c r="G12">
-        <v>1665.98195354688</v>
+        <v>1512.9609535468801</v>
       </c>
       <c r="H12">
-        <v>526.18091783743887</v>
+        <v>415.93291783743882</v>
       </c>
       <c r="I12">
         <v>251.6040694504666</v>
@@ -813,7 +813,7 @@
         <v>170.98390238990191</v>
       </c>
       <c r="C13">
-        <v>226.09143780901999</v>
+        <v>247.744304662177</v>
       </c>
       <c r="D13">
         <v>2144.5772952143848</v>
@@ -822,13 +822,13 @@
         <v>105.0221940515036</v>
       </c>
       <c r="F13">
-        <v>1536.385754778594</v>
+        <v>1532.578754778594</v>
       </c>
       <c r="G13">
-        <v>1537.7289938823201</v>
+        <v>1522.99399388232</v>
       </c>
       <c r="H13">
-        <v>430.58968059970891</v>
+        <v>417.86368059970891</v>
       </c>
       <c r="I13">
         <v>265.27969850165113</v>
@@ -842,7 +842,7 @@
         <v>169.09078529247299</v>
       </c>
       <c r="C14">
-        <v>236.37374708214861</v>
+        <v>267.06071050261841</v>
       </c>
       <c r="D14">
         <v>2167.3231107185511</v>
@@ -851,13 +851,13 @@
         <v>106.1360804360461</v>
       </c>
       <c r="F14">
-        <v>1549.204353790391</v>
+        <v>1545.397353790391</v>
       </c>
       <c r="G14">
-        <v>1541.2608178749949</v>
+        <v>1526.525817874995</v>
       </c>
       <c r="H14">
-        <v>432.52663170416571</v>
+        <v>419.80063170416571</v>
       </c>
       <c r="I14">
         <v>279.09879389494898</v>
@@ -871,7 +871,7 @@
         <v>167.19766819504409</v>
       </c>
       <c r="C15">
-        <v>255.74027715387331</v>
+        <v>286.79894046161343</v>
       </c>
       <c r="D15">
         <v>2191.2429616171412</v>
@@ -880,13 +880,13 @@
         <v>107.30746056226521</v>
       </c>
       <c r="F15">
-        <v>1562.0229528021889</v>
+        <v>1558.2159528021889</v>
       </c>
       <c r="G15">
-        <v>1537.318273222138</v>
+        <v>1522.5832732221379</v>
       </c>
       <c r="H15">
-        <v>434.48214783518279</v>
+        <v>421.75614783518279</v>
       </c>
       <c r="I15">
         <v>293.05961551598227</v>
@@ -900,7 +900,7 @@
         <v>168.18650468764571</v>
       </c>
       <c r="C16">
-        <v>263.44759160026678</v>
+        <v>294.89122979125102</v>
       </c>
       <c r="D16">
         <v>2215.8977049000259</v>
@@ -909,13 +909,13 @@
         <v>108.5148291374726</v>
       </c>
       <c r="F16">
-        <v>1572.589547736397</v>
+        <v>1568.782547736397</v>
       </c>
       <c r="G16">
-        <v>1545.0206025699781</v>
+        <v>1530.285602569978</v>
       </c>
       <c r="H16">
-        <v>436.4562289927602</v>
+        <v>423.7302289927602</v>
       </c>
       <c r="I16">
         <v>298.02592203707633</v>
@@ -929,7 +929,7 @@
         <v>169.1753411802471</v>
       </c>
       <c r="C17">
-        <v>271.56345516923977</v>
+        <v>303.40534323944189</v>
       </c>
       <c r="D17">
         <v>2239.1633223345489</v>
@@ -938,13 +938,13 @@
         <v>109.6541707664215</v>
       </c>
       <c r="F17">
-        <v>1580.1431426706049</v>
+        <v>1579.349142670605</v>
       </c>
       <c r="G17">
-        <v>1545.1543350641321</v>
+        <v>1538.937335064132</v>
       </c>
       <c r="H17">
-        <v>427.08168683471098</v>
+        <v>425.71668683471103</v>
       </c>
       <c r="I17">
         <v>303.15281641427401</v>
@@ -958,7 +958,7 @@
         <v>170.1641776728485</v>
       </c>
       <c r="C18">
-        <v>280.05072703146732</v>
+        <v>312.30293315904561</v>
       </c>
       <c r="D18">
         <v>2263.8359898219292</v>
@@ -967,13 +967,13 @@
         <v>110.8624171086775</v>
       </c>
       <c r="F18">
-        <v>1590.709737604813</v>
+        <v>1589.9157376048131</v>
       </c>
       <c r="G18">
-        <v>1553.4099515766361</v>
+        <v>1547.192951576636</v>
       </c>
       <c r="H18">
-        <v>429.06401911520402</v>
+        <v>427.69901911520401</v>
       </c>
       <c r="I18">
         <v>308.34003676535349</v>
@@ -987,7 +987,7 @@
         <v>171.15301416545</v>
       </c>
       <c r="C19">
-        <v>288.01802728313891</v>
+        <v>320.66365601867182</v>
       </c>
       <c r="D19">
         <v>2288.696861456508</v>
@@ -996,13 +996,13 @@
         <v>112.07988000494259</v>
       </c>
       <c r="F19">
-        <v>1601.276332539021</v>
+        <v>1600.4823325390209</v>
       </c>
       <c r="G19">
-        <v>1562.1978389633259</v>
+        <v>1555.9808389633261</v>
       </c>
       <c r="H19">
-        <v>431.05253973788388</v>
+        <v>429.68753973788392</v>
       </c>
       <c r="I19">
         <v>313.62925193845189</v>
@@ -1016,7 +1016,7 @@
         <v>173.69648926200901</v>
       </c>
       <c r="C20">
-        <v>288.91839029917872</v>
+        <v>321.93933937542943</v>
       </c>
       <c r="D20">
         <v>2314.5704506450529</v>
@@ -1025,13 +1025,13 @@
         <v>113.3469367394478</v>
       </c>
       <c r="F20">
-        <v>1640.712675451804</v>
+        <v>1639.9186754518039</v>
       </c>
       <c r="G20">
-        <v>1598.3725871791</v>
+        <v>1592.1555871790999</v>
       </c>
       <c r="H20">
-        <v>433.04518592202157</v>
+        <v>431.68018592202162</v>
       </c>
       <c r="I20">
         <v>314.05502117082477</v>
@@ -1045,7 +1045,7 @@
         <v>176.23996435856819</v>
       </c>
       <c r="C21">
-        <v>289.78161248589288</v>
+        <v>323.17667508504508</v>
       </c>
       <c r="D21">
         <v>2339.8704652897591</v>
@@ -1054,13 +1054,13 @@
         <v>114.58590492840121</v>
       </c>
       <c r="F21">
-        <v>1676.695018364587</v>
+        <v>1679.3550183645871</v>
       </c>
       <c r="G21">
-        <v>1627.3015946783901</v>
+        <v>1622.7235946783901</v>
       </c>
       <c r="H21">
-        <v>432.76976932543027</v>
+        <v>433.67076932543029</v>
       </c>
       <c r="I21">
         <v>314.5186220365847</v>
@@ -1074,7 +1074,7 @@
         <v>178.78343945512711</v>
       </c>
       <c r="C22">
-        <v>290.60769384328211</v>
+        <v>324.3756631475203</v>
       </c>
       <c r="D22">
         <v>2365.3049114681771</v>
@@ -1083,13 +1083,13 @@
         <v>115.83145637021821</v>
       </c>
       <c r="F22">
-        <v>1716.131361277369</v>
+        <v>1718.7913612773691</v>
       </c>
       <c r="G22">
-        <v>1650.8297581859961</v>
+        <v>1646.2517581859961</v>
       </c>
       <c r="H22">
-        <v>434.73559936009212</v>
+        <v>435.63659936009208</v>
       </c>
       <c r="I22">
         <v>315.03063898617683</v>
@@ -1103,7 +1103,7 @@
         <v>181.3269145516862</v>
       </c>
       <c r="C23">
-        <v>291.43377520067099</v>
+        <v>325.57465120999512</v>
       </c>
       <c r="D23">
         <v>2390.1837073072502</v>
@@ -1112,13 +1112,13 @@
         <v>117.0497970335318</v>
       </c>
       <c r="F23">
-        <v>1755.567704190152</v>
+        <v>1758.2277041901521</v>
       </c>
       <c r="G23">
-        <v>1667.9976210501891</v>
+        <v>1663.4196210501891</v>
       </c>
       <c r="H23">
-        <v>436.6869899296513</v>
+        <v>437.58798992965131</v>
       </c>
       <c r="I23">
         <v>315.58362470772079</v>
@@ -1132,7 +1132,7 @@
         <v>183.85985203007041</v>
       </c>
       <c r="C24">
-        <v>292.30398131342662</v>
+        <v>326.81776402783669</v>
       </c>
       <c r="D24">
         <v>2414.937033714858</v>
@@ -1141,13 +1141,13 @@
         <v>118.261993327506</v>
       </c>
       <c r="F24">
-        <v>1784.9596955994989</v>
+        <v>1787.619695599499</v>
       </c>
       <c r="G24">
-        <v>1676.0086991660939</v>
+        <v>1671.430699166094</v>
       </c>
       <c r="H24">
-        <v>438.6239410341081</v>
+        <v>439.52494103410811</v>
       </c>
       <c r="I24">
         <v>316.2395853229205</v>
@@ -1161,7 +1161,7 @@
         <v>186.3927895084546</v>
       </c>
       <c r="C25">
-        <v>293.17418742618202</v>
+        <v>328.06087684567802</v>
       </c>
       <c r="D25">
         <v>2439.8964884741581</v>
@@ -1190,7 +1190,7 @@
         <v>188.9257269868389</v>
       </c>
       <c r="C26">
-        <v>294.08153436826302</v>
+        <v>329.34233731066053</v>
       </c>
       <c r="D26">
         <v>2464.336141303103</v>
@@ -1219,7 +1219,7 @@
         <v>191.45866446522299</v>
       </c>
       <c r="C27">
-        <v>294.98888131034357</v>
+        <v>330.62379777564308</v>
       </c>
       <c r="D27">
         <v>2488.5158931668711</v>
@@ -1248,7 +1248,7 @@
         <v>194.36254309952051</v>
       </c>
       <c r="C28">
-        <v>294.38010652389193</v>
+        <v>330.39034332990889</v>
       </c>
       <c r="D28">
         <v>2512.2565020205111</v>
@@ -1277,7 +1277,7 @@
         <v>197.26642173381791</v>
       </c>
       <c r="C29">
-        <v>293.77133173744051</v>
+        <v>330.15688888417498</v>
       </c>
       <c r="D29">
         <v>2535.665513090993</v>
@@ -1306,7 +1306,7 @@
         <v>200.17030036811531</v>
       </c>
       <c r="C30">
-        <v>293.1996977803143</v>
+        <v>329.96178208558229</v>
       </c>
       <c r="D30">
         <v>2559.083486263723</v>
@@ -1335,7 +1335,7 @@
         <v>203.07417900241259</v>
       </c>
       <c r="C31">
-        <v>292.66520465251352</v>
+        <v>329.80502293413088</v>
       </c>
       <c r="D31">
         <v>2582.8330572196101</v>
@@ -1364,7 +1364,7 @@
         <v>206.00159731602</v>
       </c>
       <c r="C32">
-        <v>292.03214251474122</v>
+        <v>329.54969477270748</v>
       </c>
       <c r="D32">
         <v>2607.0934680036062</v>
@@ -1393,7 +1393,7 @@
         <v>208.92901562962729</v>
       </c>
       <c r="C33">
-        <v>291.39908037696858</v>
+        <v>329.2943666112842</v>
       </c>
       <c r="D33">
         <v>2631.766135490986</v>
@@ -1422,7 +1422,7 @@
         <v>211.85643394323469</v>
       </c>
       <c r="C34">
-        <v>290.80315906852138</v>
+        <v>329.07738609700209</v>
       </c>
       <c r="D34">
         <v>2656.7704007615239</v>
@@ -1451,7 +1451,7 @@
         <v>214.7838522568419</v>
       </c>
       <c r="C35">
-        <v>290.20723776007452</v>
+        <v>328.86040558272009</v>
       </c>
       <c r="D35">
         <v>2681.7298555208249</v>
@@ -1480,7 +1480,7 @@
         <v>217.8087435385666</v>
       </c>
       <c r="C36">
-        <v>289.24030329381378</v>
+        <v>328.27361872844011</v>
       </c>
       <c r="D36">
         <v>2706.7878934048481</v>
@@ -1509,7 +1509,7 @@
         <v>220.83363482029131</v>
       </c>
       <c r="C37">
-        <v>288.27336882755282</v>
+        <v>327.68683187415991</v>
       </c>
       <c r="D37">
         <v>2731.9265902090979</v>
@@ -1538,7 +1538,7 @@
         <v>223.85852610201621</v>
       </c>
       <c r="C38">
-        <v>287.30643436129151</v>
+        <v>327.1000450198793</v>
       </c>
       <c r="D38">
         <v>2757.0204765021122</v>
@@ -1567,7 +1567,7 @@
         <v>226.88341738374069</v>
       </c>
       <c r="C39">
-        <v>286.37664072435621</v>
+        <v>326.551605812741</v>
       </c>
       <c r="D39">
         <v>2782.0157796704029</v>
@@ -1596,7 +1596,7 @@
         <v>230.0749559980533</v>
       </c>
       <c r="C40">
-        <v>284.82331709063999</v>
+        <v>325.38205024445301</v>
       </c>
       <c r="D40">
         <v>2807.2440974971282</v>
@@ -1625,7 +1625,7 @@
         <v>233.2664946123657</v>
       </c>
       <c r="C41">
-        <v>283.30713428624921</v>
+        <v>324.25084232330607</v>
       </c>
       <c r="D41">
         <v>2832.5441121418339</v>
@@ -1654,7 +1654,7 @@
         <v>236.45803322667831</v>
       </c>
       <c r="C42">
-        <v>281.86523314050908</v>
+        <v>323.19632969644169</v>
       </c>
       <c r="D42">
         <v>2858.1488382629541</v>
@@ -1683,7 +1683,7 @@
         <v>239.6495718409908</v>
       </c>
       <c r="C43">
-        <v>280.49761365341982</v>
+        <v>322.21851236385947</v>
       </c>
       <c r="D43">
         <v>2884.2464800076882</v>
@@ -1712,7 +1712,7 @@
         <v>242.96586225756681</v>
       </c>
       <c r="C44">
-        <v>278.68189565661112</v>
+        <v>320.79501015719001</v>
       </c>
       <c r="D44">
         <v>2910.8011889670452</v>
@@ -1741,7 +1741,7 @@
         <v>246.28215267414279</v>
       </c>
       <c r="C45">
-        <v>276.94045931845392</v>
+        <v>319.44820324480298</v>
       </c>
       <c r="D45">
         <v>2937.8756998567569</v>
@@ -1770,7 +1770,7 @@
         <v>249.59844309071909</v>
       </c>
       <c r="C46">
-        <v>275.31044546827241</v>
+        <v>318.21643927383991</v>
       </c>
       <c r="D46">
         <v>2965.0487938711908</v>
@@ -1799,7 +1799,7 @@
         <v>252.91473350729501</v>
       </c>
       <c r="C47">
-        <v>273.7175724474165</v>
+        <v>317.02302295001772</v>
       </c>
       <c r="D47">
         <v>2992.3742436238322</v>
@@ -1826,13 +1826,1303 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{739C81E1-ABA7-4289-AEC8-FA80445C03F1}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDD24C66-168E-4D76-8E03-01544E0E1730}">
+  <dimension ref="A1:AU9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AU9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>44012</v>
+      </c>
+      <c r="C1" s="2">
+        <v>44104</v>
+      </c>
+      <c r="D1" s="2">
+        <v>44196</v>
+      </c>
+      <c r="E1" s="2">
+        <v>44286</v>
+      </c>
+      <c r="F1" s="2">
+        <v>44377</v>
+      </c>
+      <c r="G1" s="2">
+        <v>44469</v>
+      </c>
+      <c r="H1" s="2">
+        <v>44561</v>
+      </c>
+      <c r="I1" s="2">
+        <v>44651</v>
+      </c>
+      <c r="J1" s="2">
+        <v>44742</v>
+      </c>
+      <c r="K1" s="2">
+        <v>44834</v>
+      </c>
+      <c r="L1" s="2">
+        <v>44926</v>
+      </c>
+      <c r="M1" s="2">
+        <v>45016</v>
+      </c>
+      <c r="N1" s="2">
+        <v>45107</v>
+      </c>
+      <c r="O1" s="2">
+        <v>45199</v>
+      </c>
+      <c r="P1" s="2">
+        <v>45291</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>45382</v>
+      </c>
+      <c r="R1" s="2">
+        <v>45473</v>
+      </c>
+      <c r="S1" s="2">
+        <v>45565</v>
+      </c>
+      <c r="T1" s="2">
+        <v>45657</v>
+      </c>
+      <c r="U1" s="2">
+        <v>45747</v>
+      </c>
+      <c r="V1" s="2">
+        <v>45838</v>
+      </c>
+      <c r="W1" s="2">
+        <v>45930</v>
+      </c>
+      <c r="X1" s="2">
+        <v>46022</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>46112</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>46203</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>46295</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>46387</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>46477</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>46568</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>46660</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>46752</v>
+      </c>
+      <c r="AG1" s="2">
+        <v>46843</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>46934</v>
+      </c>
+      <c r="AI1" s="2">
+        <v>47026</v>
+      </c>
+      <c r="AJ1" s="2">
+        <v>47118</v>
+      </c>
+      <c r="AK1" s="2">
+        <v>47208</v>
+      </c>
+      <c r="AL1" s="2">
+        <v>47299</v>
+      </c>
+      <c r="AM1" s="2">
+        <v>47391</v>
+      </c>
+      <c r="AN1" s="2">
+        <v>47483</v>
+      </c>
+      <c r="AO1" s="2">
+        <v>47573</v>
+      </c>
+      <c r="AP1" s="2">
+        <v>47664</v>
+      </c>
+      <c r="AQ1" s="2">
+        <v>47756</v>
+      </c>
+      <c r="AR1" s="2">
+        <v>47848</v>
+      </c>
+      <c r="AS1" s="2">
+        <v>47938</v>
+      </c>
+      <c r="AT1" s="2">
+        <v>48029</v>
+      </c>
+      <c r="AU1" s="2">
+        <v>48121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>156.16</v>
+      </c>
+      <c r="C2">
+        <v>197.62799999999999</v>
+      </c>
+      <c r="D2">
+        <v>170.20699999999999</v>
+      </c>
+      <c r="E2">
+        <v>164.13699999999989</v>
+      </c>
+      <c r="F2">
+        <v>168.2833827902208</v>
+      </c>
+      <c r="G2">
+        <v>172.42976558044171</v>
+      </c>
+      <c r="H2">
+        <v>173.0148583315212</v>
+      </c>
+      <c r="I2">
+        <v>173.59995108260071</v>
+      </c>
+      <c r="J2">
+        <v>174.1850438336802</v>
+      </c>
+      <c r="K2">
+        <v>174.77013658475971</v>
+      </c>
+      <c r="L2">
+        <v>172.87701948733081</v>
+      </c>
+      <c r="M2">
+        <v>170.98390238990191</v>
+      </c>
+      <c r="N2">
+        <v>169.09078529247299</v>
+      </c>
+      <c r="O2">
+        <v>167.19766819504409</v>
+      </c>
+      <c r="P2">
+        <v>168.18650468764571</v>
+      </c>
+      <c r="Q2">
+        <v>169.1753411802471</v>
+      </c>
+      <c r="R2">
+        <v>170.1641776728485</v>
+      </c>
+      <c r="S2">
+        <v>171.15301416545</v>
+      </c>
+      <c r="T2">
+        <v>173.69648926200901</v>
+      </c>
+      <c r="U2">
+        <v>176.23996435856819</v>
+      </c>
+      <c r="V2">
+        <v>178.78343945512711</v>
+      </c>
+      <c r="W2">
+        <v>181.3269145516862</v>
+      </c>
+      <c r="X2">
+        <v>183.85985203007041</v>
+      </c>
+      <c r="Y2">
+        <v>186.3927895084546</v>
+      </c>
+      <c r="Z2">
+        <v>188.9257269868389</v>
+      </c>
+      <c r="AA2">
+        <v>191.45866446522299</v>
+      </c>
+      <c r="AB2">
+        <v>194.36254309952051</v>
+      </c>
+      <c r="AC2">
+        <v>197.26642173381791</v>
+      </c>
+      <c r="AD2">
+        <v>200.17030036811531</v>
+      </c>
+      <c r="AE2">
+        <v>203.07417900241259</v>
+      </c>
+      <c r="AF2">
+        <v>206.00159731602</v>
+      </c>
+      <c r="AG2">
+        <v>208.92901562962729</v>
+      </c>
+      <c r="AH2">
+        <v>211.85643394323469</v>
+      </c>
+      <c r="AI2">
+        <v>214.7838522568419</v>
+      </c>
+      <c r="AJ2">
+        <v>217.8087435385666</v>
+      </c>
+      <c r="AK2">
+        <v>220.83363482029131</v>
+      </c>
+      <c r="AL2">
+        <v>223.85852610201621</v>
+      </c>
+      <c r="AM2">
+        <v>226.88341738374069</v>
+      </c>
+      <c r="AN2">
+        <v>230.0749559980533</v>
+      </c>
+      <c r="AO2">
+        <v>233.2664946123657</v>
+      </c>
+      <c r="AP2">
+        <v>236.45803322667831</v>
+      </c>
+      <c r="AQ2">
+        <v>239.6495718409908</v>
+      </c>
+      <c r="AR2">
+        <v>242.96586225756681</v>
+      </c>
+      <c r="AS2">
+        <v>246.28215267414279</v>
+      </c>
+      <c r="AT2">
+        <v>249.59844309071909</v>
+      </c>
+      <c r="AU2">
+        <v>252.91473350729501</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>440</v>
+      </c>
+      <c r="C3">
+        <v>363.8</v>
+      </c>
+      <c r="D3">
+        <v>243.1</v>
+      </c>
+      <c r="E3">
+        <v>216.8</v>
+      </c>
+      <c r="F3">
+        <v>201.69787045292151</v>
+      </c>
+      <c r="G3">
+        <v>188.86729215584299</v>
+      </c>
+      <c r="H3">
+        <v>193.24899108297839</v>
+      </c>
+      <c r="I3">
+        <v>199.97623704208269</v>
+      </c>
+      <c r="J3">
+        <v>205.88603266163159</v>
+      </c>
+      <c r="K3">
+        <v>212.3326953411578</v>
+      </c>
+      <c r="L3">
+        <v>229.53998058883141</v>
+      </c>
+      <c r="M3">
+        <v>247.744304662177</v>
+      </c>
+      <c r="N3">
+        <v>267.06071050261841</v>
+      </c>
+      <c r="O3">
+        <v>286.79894046161343</v>
+      </c>
+      <c r="P3">
+        <v>294.89122979125102</v>
+      </c>
+      <c r="Q3">
+        <v>303.40534323944189</v>
+      </c>
+      <c r="R3">
+        <v>312.30293315904561</v>
+      </c>
+      <c r="S3">
+        <v>320.66365601867182</v>
+      </c>
+      <c r="T3">
+        <v>321.93933937542943</v>
+      </c>
+      <c r="U3">
+        <v>323.17667508504508</v>
+      </c>
+      <c r="V3">
+        <v>324.3756631475203</v>
+      </c>
+      <c r="W3">
+        <v>325.57465120999512</v>
+      </c>
+      <c r="X3">
+        <v>326.81776402783669</v>
+      </c>
+      <c r="Y3">
+        <v>328.06087684567802</v>
+      </c>
+      <c r="Z3">
+        <v>329.34233731066053</v>
+      </c>
+      <c r="AA3">
+        <v>330.62379777564308</v>
+      </c>
+      <c r="AB3">
+        <v>330.39034332990889</v>
+      </c>
+      <c r="AC3">
+        <v>330.15688888417498</v>
+      </c>
+      <c r="AD3">
+        <v>329.96178208558229</v>
+      </c>
+      <c r="AE3">
+        <v>329.80502293413088</v>
+      </c>
+      <c r="AF3">
+        <v>329.54969477270748</v>
+      </c>
+      <c r="AG3">
+        <v>329.2943666112842</v>
+      </c>
+      <c r="AH3">
+        <v>329.07738609700209</v>
+      </c>
+      <c r="AI3">
+        <v>328.86040558272009</v>
+      </c>
+      <c r="AJ3">
+        <v>328.27361872844011</v>
+      </c>
+      <c r="AK3">
+        <v>327.68683187415991</v>
+      </c>
+      <c r="AL3">
+        <v>327.1000450198793</v>
+      </c>
+      <c r="AM3">
+        <v>326.551605812741</v>
+      </c>
+      <c r="AN3">
+        <v>325.38205024445301</v>
+      </c>
+      <c r="AO3">
+        <v>324.25084232330607</v>
+      </c>
+      <c r="AP3">
+        <v>323.19632969644169</v>
+      </c>
+      <c r="AQ3">
+        <v>322.21851236385947</v>
+      </c>
+      <c r="AR3">
+        <v>320.79501015719001</v>
+      </c>
+      <c r="AS3">
+        <v>319.44820324480298</v>
+      </c>
+      <c r="AT3">
+        <v>318.21643927383991</v>
+      </c>
+      <c r="AU3">
+        <v>317.02302295001772</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1779.8</v>
+      </c>
+      <c r="C4">
+        <v>1871.3</v>
+      </c>
+      <c r="D4">
+        <v>1907.1</v>
+      </c>
+      <c r="E4">
+        <v>1958.3</v>
+      </c>
+      <c r="F4">
+        <v>1978.3751090344099</v>
+      </c>
+      <c r="G4">
+        <v>2007.0179878174349</v>
+      </c>
+      <c r="H4">
+        <v>2033.6981662082569</v>
+      </c>
+      <c r="I4">
+        <v>2058.944408239478</v>
+      </c>
+      <c r="J4">
+        <v>2079.7902580671739</v>
+      </c>
+      <c r="K4">
+        <v>2102.1686273791929</v>
+      </c>
+      <c r="L4">
+        <v>2124.2512473170441</v>
+      </c>
+      <c r="M4">
+        <v>2144.5772952143848</v>
+      </c>
+      <c r="N4">
+        <v>2167.3231107185511</v>
+      </c>
+      <c r="O4">
+        <v>2191.2429616171412</v>
+      </c>
+      <c r="P4">
+        <v>2215.8977049000259</v>
+      </c>
+      <c r="Q4">
+        <v>2239.1633223345489</v>
+      </c>
+      <c r="R4">
+        <v>2263.8359898219292</v>
+      </c>
+      <c r="S4">
+        <v>2288.696861456508</v>
+      </c>
+      <c r="T4">
+        <v>2314.5704506450529</v>
+      </c>
+      <c r="U4">
+        <v>2339.8704652897591</v>
+      </c>
+      <c r="V4">
+        <v>2365.3049114681771</v>
+      </c>
+      <c r="W4">
+        <v>2390.1837073072502</v>
+      </c>
+      <c r="X4">
+        <v>2414.937033714858</v>
+      </c>
+      <c r="Y4">
+        <v>2439.8964884741581</v>
+      </c>
+      <c r="Z4">
+        <v>2464.336141303103</v>
+      </c>
+      <c r="AA4">
+        <v>2488.5158931668711</v>
+      </c>
+      <c r="AB4">
+        <v>2512.2565020205111</v>
+      </c>
+      <c r="AC4">
+        <v>2535.665513090993</v>
+      </c>
+      <c r="AD4">
+        <v>2559.083486263723</v>
+      </c>
+      <c r="AE4">
+        <v>2582.8330572196101</v>
+      </c>
+      <c r="AF4">
+        <v>2607.0934680036062</v>
+      </c>
+      <c r="AG4">
+        <v>2631.766135490986</v>
+      </c>
+      <c r="AH4">
+        <v>2656.7704007615239</v>
+      </c>
+      <c r="AI4">
+        <v>2681.7298555208249</v>
+      </c>
+      <c r="AJ4">
+        <v>2706.7878934048481</v>
+      </c>
+      <c r="AK4">
+        <v>2731.9265902090979</v>
+      </c>
+      <c r="AL4">
+        <v>2757.0204765021122</v>
+      </c>
+      <c r="AM4">
+        <v>2782.0157796704029</v>
+      </c>
+      <c r="AN4">
+        <v>2807.2440974971282</v>
+      </c>
+      <c r="AO4">
+        <v>2832.5441121418339</v>
+      </c>
+      <c r="AP4">
+        <v>2858.1488382629541</v>
+      </c>
+      <c r="AQ4">
+        <v>2884.2464800076882</v>
+      </c>
+      <c r="AR4">
+        <v>2910.8011889670452</v>
+      </c>
+      <c r="AS4">
+        <v>2937.8756998567569</v>
+      </c>
+      <c r="AT4">
+        <v>2965.0487938711908</v>
+      </c>
+      <c r="AU4">
+        <v>2992.3742436238322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>54.2</v>
+      </c>
+      <c r="C5">
+        <v>90.2</v>
+      </c>
+      <c r="D5">
+        <v>95.9</v>
+      </c>
+      <c r="E5">
+        <v>95.9</v>
+      </c>
+      <c r="F5">
+        <v>96.883099094316492</v>
+      </c>
+      <c r="G5">
+        <v>98.285770837814454</v>
+      </c>
+      <c r="H5">
+        <v>99.592327089502035</v>
+      </c>
+      <c r="I5">
+        <v>100.82866197730991</v>
+      </c>
+      <c r="J5">
+        <v>101.8495050547117</v>
+      </c>
+      <c r="K5">
+        <v>102.94539721476001</v>
+      </c>
+      <c r="L5">
+        <v>104.0268062185081</v>
+      </c>
+      <c r="M5">
+        <v>105.0221940515036</v>
+      </c>
+      <c r="N5">
+        <v>106.1360804360461</v>
+      </c>
+      <c r="O5">
+        <v>107.30746056226521</v>
+      </c>
+      <c r="P5">
+        <v>108.5148291374726</v>
+      </c>
+      <c r="Q5">
+        <v>109.6541707664215</v>
+      </c>
+      <c r="R5">
+        <v>110.8624171086775</v>
+      </c>
+      <c r="S5">
+        <v>112.07988000494259</v>
+      </c>
+      <c r="T5">
+        <v>113.3469367394478</v>
+      </c>
+      <c r="U5">
+        <v>114.58590492840121</v>
+      </c>
+      <c r="V5">
+        <v>115.83145637021821</v>
+      </c>
+      <c r="W5">
+        <v>117.0497970335318</v>
+      </c>
+      <c r="X5">
+        <v>118.261993327506</v>
+      </c>
+      <c r="Y5">
+        <v>119.4842839425379</v>
+      </c>
+      <c r="Z5">
+        <v>120.68111931316329</v>
+      </c>
+      <c r="AA5">
+        <v>121.8652270615856</v>
+      </c>
+      <c r="AB5">
+        <v>123.0278295173197</v>
+      </c>
+      <c r="AC5">
+        <v>124.1741932826566</v>
+      </c>
+      <c r="AD5">
+        <v>125.3209959315177</v>
+      </c>
+      <c r="AE5">
+        <v>126.4840372707761</v>
+      </c>
+      <c r="AF5">
+        <v>127.6720949709166</v>
+      </c>
+      <c r="AG5">
+        <v>128.88034131317249</v>
+      </c>
+      <c r="AH5">
+        <v>130.10482634582559</v>
+      </c>
+      <c r="AI5">
+        <v>131.3271169608575</v>
+      </c>
+      <c r="AJ5">
+        <v>132.55423529465611</v>
+      </c>
+      <c r="AK5">
+        <v>133.78530358017301</v>
+      </c>
+      <c r="AL5">
+        <v>135.01417744806861</v>
+      </c>
+      <c r="AM5">
+        <v>136.23822359719739</v>
+      </c>
+      <c r="AN5">
+        <v>137.47368071795671</v>
+      </c>
+      <c r="AO5">
+        <v>138.71264890691</v>
+      </c>
+      <c r="AP5">
+        <v>139.96653913568781</v>
+      </c>
+      <c r="AQ5">
+        <v>141.24456795829931</v>
+      </c>
+      <c r="AR5">
+        <v>142.54497984064739</v>
+      </c>
+      <c r="AS5">
+        <v>143.8708469674018</v>
+      </c>
+      <c r="AT5">
+        <v>145.2015418129231</v>
+      </c>
+      <c r="AU5">
+        <v>146.53969767835659</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1336.74</v>
+      </c>
+      <c r="C6">
+        <v>1328.7719999999999</v>
+      </c>
+      <c r="D6">
+        <v>1372.7929999999999</v>
+      </c>
+      <c r="E6">
+        <v>1403.2629999999999</v>
+      </c>
+      <c r="F6">
+        <v>1394.63952711825</v>
+      </c>
+      <c r="G6">
+        <v>1386.0160542364999</v>
+      </c>
+      <c r="H6">
+        <v>1416.247429866125</v>
+      </c>
+      <c r="I6">
+        <v>1446.4788054957489</v>
+      </c>
+      <c r="J6">
+        <v>1476.710181125374</v>
+      </c>
+      <c r="K6">
+        <v>1506.9415567549979</v>
+      </c>
+      <c r="L6">
+        <v>1519.7601557667949</v>
+      </c>
+      <c r="M6">
+        <v>1532.578754778594</v>
+      </c>
+      <c r="N6">
+        <v>1545.397353790391</v>
+      </c>
+      <c r="O6">
+        <v>1558.2159528021889</v>
+      </c>
+      <c r="P6">
+        <v>1568.782547736397</v>
+      </c>
+      <c r="Q6">
+        <v>1579.349142670605</v>
+      </c>
+      <c r="R6">
+        <v>1589.9157376048131</v>
+      </c>
+      <c r="S6">
+        <v>1600.4823325390209</v>
+      </c>
+      <c r="T6">
+        <v>1639.9186754518039</v>
+      </c>
+      <c r="U6">
+        <v>1679.3550183645871</v>
+      </c>
+      <c r="V6">
+        <v>1718.7913612773691</v>
+      </c>
+      <c r="W6">
+        <v>1758.2277041901521</v>
+      </c>
+      <c r="X6">
+        <v>1787.619695599499</v>
+      </c>
+      <c r="Y6">
+        <v>1817.0116870088459</v>
+      </c>
+      <c r="Z6">
+        <v>1846.403678418194</v>
+      </c>
+      <c r="AA6">
+        <v>1875.7956698275409</v>
+      </c>
+      <c r="AB6">
+        <v>1908.214872793631</v>
+      </c>
+      <c r="AC6">
+        <v>1940.63407575972</v>
+      </c>
+      <c r="AD6">
+        <v>1973.0532787258101</v>
+      </c>
+      <c r="AE6">
+        <v>2005.472481691899</v>
+      </c>
+      <c r="AF6">
+        <v>2057.1759873287519</v>
+      </c>
+      <c r="AG6">
+        <v>2108.879492965606</v>
+      </c>
+      <c r="AH6">
+        <v>2160.5829986024601</v>
+      </c>
+      <c r="AI6">
+        <v>2212.2865042393132</v>
+      </c>
+      <c r="AJ6">
+        <v>2211.5343138466092</v>
+      </c>
+      <c r="AK6">
+        <v>2210.7821234539051</v>
+      </c>
+      <c r="AL6">
+        <v>2210.0299330612011</v>
+      </c>
+      <c r="AM6">
+        <v>2209.2777426684961</v>
+      </c>
+      <c r="AN6">
+        <v>2261.6493087725662</v>
+      </c>
+      <c r="AO6">
+        <v>2314.0208748766349</v>
+      </c>
+      <c r="AP6">
+        <v>2366.392440980705</v>
+      </c>
+      <c r="AQ6">
+        <v>2418.7640070847742</v>
+      </c>
+      <c r="AR6">
+        <v>2464.3652051309859</v>
+      </c>
+      <c r="AS6">
+        <v>2509.9664031771981</v>
+      </c>
+      <c r="AT6">
+        <v>2555.5676012234089</v>
+      </c>
+      <c r="AU6">
+        <v>2601.1687992696211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1828.5000000000009</v>
+      </c>
+      <c r="C7">
+        <v>1861.4</v>
+      </c>
+      <c r="D7">
+        <v>1756.1999999999989</v>
+      </c>
+      <c r="E7">
+        <v>1808.7</v>
+      </c>
+      <c r="F7">
+        <v>1629.356357104331</v>
+      </c>
+      <c r="G7">
+        <v>1501.6652887165669</v>
+      </c>
+      <c r="H7">
+        <v>1514.272945247701</v>
+      </c>
+      <c r="I7">
+        <v>1515.6150242949509</v>
+      </c>
+      <c r="J7">
+        <v>1509.926416318757</v>
+      </c>
+      <c r="K7">
+        <v>1493.7178340556329</v>
+      </c>
+      <c r="L7">
+        <v>1512.9609535468801</v>
+      </c>
+      <c r="M7">
+        <v>1522.99399388232</v>
+      </c>
+      <c r="N7">
+        <v>1526.525817874995</v>
+      </c>
+      <c r="O7">
+        <v>1522.5832732221379</v>
+      </c>
+      <c r="P7">
+        <v>1530.285602569978</v>
+      </c>
+      <c r="Q7">
+        <v>1538.937335064132</v>
+      </c>
+      <c r="R7">
+        <v>1547.192951576636</v>
+      </c>
+      <c r="S7">
+        <v>1555.9808389633261</v>
+      </c>
+      <c r="T7">
+        <v>1592.1555871790999</v>
+      </c>
+      <c r="U7">
+        <v>1622.7235946783901</v>
+      </c>
+      <c r="V7">
+        <v>1646.2517581859961</v>
+      </c>
+      <c r="W7">
+        <v>1663.4196210501891</v>
+      </c>
+      <c r="X7">
+        <v>1671.430699166094</v>
+      </c>
+      <c r="Y7">
+        <v>1682.1431104472849</v>
+      </c>
+      <c r="Z7">
+        <v>1694.6607802102719</v>
+      </c>
+      <c r="AA7">
+        <v>1709.3896382183029</v>
+      </c>
+      <c r="AB7">
+        <v>1722.372615576626</v>
+      </c>
+      <c r="AC7">
+        <v>1735.0429474429729</v>
+      </c>
+      <c r="AD7">
+        <v>1746.4953393081139</v>
+      </c>
+      <c r="AE7">
+        <v>1757.1882121565191</v>
+      </c>
+      <c r="AF7">
+        <v>1788.9509959744839</v>
+      </c>
+      <c r="AG7">
+        <v>1816.7189541257289</v>
+      </c>
+      <c r="AH7">
+        <v>1839.6922791598031</v>
+      </c>
+      <c r="AI7">
+        <v>1858.259733230635</v>
+      </c>
+      <c r="AJ7">
+        <v>1832.4294189532291</v>
+      </c>
+      <c r="AK7">
+        <v>1818.576749321116</v>
+      </c>
+      <c r="AL7">
+        <v>1816.4404652627579</v>
+      </c>
+      <c r="AM7">
+        <v>1826.107622074454</v>
+      </c>
+      <c r="AN7">
+        <v>1883.521840106393</v>
+      </c>
+      <c r="AO7">
+        <v>1928.497184954686</v>
+      </c>
+      <c r="AP7">
+        <v>1962.138859372219</v>
+      </c>
+      <c r="AQ7">
+        <v>1983.801049724259</v>
+      </c>
+      <c r="AR7">
+        <v>1944.7885028241169</v>
+      </c>
+      <c r="AS7">
+        <v>1906.4485972733521</v>
+      </c>
+      <c r="AT7">
+        <v>1870.239333659976</v>
+      </c>
+      <c r="AU7">
+        <v>1835.4218257479581</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1085.9000000000001</v>
+      </c>
+      <c r="C8">
+        <v>1212.9000000000001</v>
+      </c>
+      <c r="D8">
+        <v>609.79999999999995</v>
+      </c>
+      <c r="E8">
+        <v>402.3</v>
+      </c>
+      <c r="F8">
+        <v>404.18538158623392</v>
+      </c>
+      <c r="G8">
+        <v>406.11408156777497</v>
+      </c>
+      <c r="H8">
+        <v>408.08197438316557</v>
+      </c>
+      <c r="I8">
+        <v>410.07255778657441</v>
+      </c>
+      <c r="J8">
+        <v>412.05076450560961</v>
+      </c>
+      <c r="K8">
+        <v>413.998029513711</v>
+      </c>
+      <c r="L8">
+        <v>415.93291783743882</v>
+      </c>
+      <c r="M8">
+        <v>417.86368059970891</v>
+      </c>
+      <c r="N8">
+        <v>419.80063170416571</v>
+      </c>
+      <c r="O8">
+        <v>421.75614783518279</v>
+      </c>
+      <c r="P8">
+        <v>423.7302289927602</v>
+      </c>
+      <c r="Q8">
+        <v>425.71668683471103</v>
+      </c>
+      <c r="R8">
+        <v>427.69901911520401</v>
+      </c>
+      <c r="S8">
+        <v>429.68753973788392</v>
+      </c>
+      <c r="T8">
+        <v>431.68018592202162</v>
+      </c>
+      <c r="U8">
+        <v>433.67076932543029</v>
+      </c>
+      <c r="V8">
+        <v>435.63659936009208</v>
+      </c>
+      <c r="W8">
+        <v>437.58798992965131</v>
+      </c>
+      <c r="X8">
+        <v>439.52494103410811</v>
+      </c>
+      <c r="Y8">
+        <v>441.44951545419133</v>
+      </c>
+      <c r="Z8">
+        <v>443.35552484771432</v>
+      </c>
+      <c r="AA8">
+        <v>445.25947146050851</v>
+      </c>
+      <c r="AB8">
+        <v>447.16548085403139</v>
+      </c>
+      <c r="AC8">
+        <v>449.0735530282833</v>
+      </c>
+      <c r="AD8">
+        <v>450.98368798326419</v>
+      </c>
+      <c r="AE8">
+        <v>452.90619962261849</v>
+      </c>
+      <c r="AF8">
+        <v>454.83283682343068</v>
+      </c>
+      <c r="AG8">
+        <v>456.76772514715861</v>
+      </c>
+      <c r="AH8">
+        <v>458.72736683963342</v>
+      </c>
+      <c r="AI8">
+        <v>460.70763633939748</v>
+      </c>
+      <c r="AJ8">
+        <v>462.71059642718001</v>
+      </c>
+      <c r="AK8">
+        <v>464.73212154152247</v>
+      </c>
+      <c r="AL8">
+        <v>466.76808612096738</v>
+      </c>
+      <c r="AM8">
+        <v>468.80198791968348</v>
+      </c>
+      <c r="AN8">
+        <v>470.83176415694169</v>
+      </c>
+      <c r="AO8">
+        <v>472.86360317492881</v>
+      </c>
+      <c r="AP8">
+        <v>474.89544219291588</v>
+      </c>
+      <c r="AQ8">
+        <v>476.92728121090312</v>
+      </c>
+      <c r="AR8">
+        <v>478.96530857107712</v>
+      </c>
+      <c r="AS8">
+        <v>481.00539871197992</v>
+      </c>
+      <c r="AT8">
+        <v>483.04961441434068</v>
+      </c>
+      <c r="AU8">
+        <v>485.09176733597252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>884.2600000000001</v>
+      </c>
+      <c r="C9">
+        <v>242.12799999999999</v>
+      </c>
+      <c r="D9">
+        <v>225.90700000000001</v>
+      </c>
+      <c r="E9">
+        <v>260.73700000000002</v>
+      </c>
+      <c r="F9">
+        <v>232.07518871317359</v>
+      </c>
+      <c r="G9">
+        <v>215.720203842161</v>
+      </c>
+      <c r="H9">
+        <v>220.89139620745101</v>
+      </c>
+      <c r="I9">
+        <v>226.76914626180869</v>
+      </c>
+      <c r="J9">
+        <v>232.32795235033251</v>
+      </c>
+      <c r="K9">
+        <v>237.9298898973548</v>
+      </c>
+      <c r="L9">
+        <v>251.6040694504666</v>
+      </c>
+      <c r="M9">
+        <v>265.27969850165113</v>
+      </c>
+      <c r="N9">
+        <v>279.09879389494898</v>
+      </c>
+      <c r="O9">
+        <v>293.05961551598227</v>
+      </c>
+      <c r="P9">
+        <v>298.02592203707633</v>
+      </c>
+      <c r="Q9">
+        <v>303.15281641427401</v>
+      </c>
+      <c r="R9">
+        <v>308.34003676535349</v>
+      </c>
+      <c r="S9">
+        <v>313.62925193845189</v>
+      </c>
+      <c r="T9">
+        <v>314.05502117082477</v>
+      </c>
+      <c r="U9">
+        <v>314.5186220365847</v>
+      </c>
+      <c r="V9">
+        <v>315.03063898617683</v>
+      </c>
+      <c r="W9">
+        <v>315.58362470772079</v>
+      </c>
+      <c r="X9">
+        <v>316.2395853229205</v>
+      </c>
+      <c r="Y9">
+        <v>316.95514017513671</v>
+      </c>
+      <c r="Z9">
+        <v>317.71048621778692</v>
+      </c>
+      <c r="AA9">
+        <v>318.55415230022101</v>
+      </c>
+      <c r="AB9">
+        <v>318.29850133827199</v>
+      </c>
+      <c r="AC9">
+        <v>318.13366691457782</v>
+      </c>
+      <c r="AD9">
+        <v>318.04565082439819</v>
+      </c>
+      <c r="AE9">
+        <v>318.06410134177349</v>
+      </c>
+      <c r="AF9">
+        <v>318.09729229239042</v>
+      </c>
+      <c r="AG9">
+        <v>318.17786928038868</v>
+      </c>
+      <c r="AH9">
+        <v>318.36379279589238</v>
+      </c>
+      <c r="AI9">
+        <v>318.64707655433722</v>
+      </c>
+      <c r="AJ9">
+        <v>318.72234084172197</v>
+      </c>
+      <c r="AK9">
+        <v>318.86952061123691</v>
+      </c>
+      <c r="AL9">
+        <v>319.10267892127462</v>
+      </c>
+      <c r="AM9">
+        <v>319.38590629755907</v>
+      </c>
+      <c r="AN9">
+        <v>319.19110945656053</v>
+      </c>
+      <c r="AO9">
+        <v>319.05567634036208</v>
+      </c>
+      <c r="AP9">
+        <v>318.97514203538952</v>
+      </c>
+      <c r="AQ9">
+        <v>318.9496051242694</v>
+      </c>
+      <c r="AR9">
+        <v>318.60334826748328</v>
+      </c>
+      <c r="AS9">
+        <v>318.31720335346819</v>
+      </c>
+      <c r="AT9">
+        <v>318.11173048290601</v>
+      </c>
+      <c r="AU9">
+        <v>317.95738112604761</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>